<commit_message>
Kinda final results I guess?
</commit_message>
<xml_diff>
--- a/wyniki/AI_statistics.xlsx
+++ b/wyniki/AI_statistics.xlsx
@@ -537,61 +537,61 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="T2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -601,61 +601,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.161290322580645</v>
+        <v>3.264705882352941</v>
       </c>
       <c r="C3" t="n">
-        <v>3.451612903225806</v>
+        <v>3.5</v>
       </c>
       <c r="D3" t="n">
-        <v>3.032258064516129</v>
+        <v>3.029411764705882</v>
       </c>
       <c r="E3" t="n">
-        <v>2.870967741935484</v>
+        <v>2.794117647058823</v>
       </c>
       <c r="F3" t="n">
-        <v>3.064516129032258</v>
+        <v>3.058823529411764</v>
       </c>
       <c r="G3" t="n">
-        <v>3.258064516129032</v>
+        <v>3.352941176470588</v>
       </c>
       <c r="H3" t="n">
-        <v>2.67741935483871</v>
+        <v>2.705882352941177</v>
       </c>
       <c r="I3" t="n">
-        <v>2.870967741935484</v>
+        <v>2.852941176470588</v>
       </c>
       <c r="J3" t="n">
-        <v>2.903225806451613</v>
+        <v>2.823529411764706</v>
       </c>
       <c r="K3" t="n">
-        <v>3.290322580645161</v>
+        <v>3.352941176470588</v>
       </c>
       <c r="L3" t="n">
-        <v>3.354838709677419</v>
+        <v>3.323529411764706</v>
       </c>
       <c r="M3" t="n">
-        <v>2.967741935483871</v>
+        <v>2.823529411764706</v>
       </c>
       <c r="N3" t="n">
-        <v>3.225806451612903</v>
+        <v>3.147058823529412</v>
       </c>
       <c r="O3" t="n">
-        <v>3.612903225806452</v>
+        <v>3.676470588235294</v>
       </c>
       <c r="P3" t="n">
-        <v>3.387096774193548</v>
+        <v>3.205882352941177</v>
       </c>
       <c r="Q3" t="n">
-        <v>3.419354838709677</v>
+        <v>3.382352941176471</v>
       </c>
       <c r="R3" t="n">
-        <v>3.258064516129032</v>
+        <v>3.323529411764706</v>
       </c>
       <c r="S3" t="n">
-        <v>3.354838709677419</v>
+        <v>3.411764705882353</v>
       </c>
       <c r="T3" t="n">
-        <v>2.774193548387097</v>
+        <v>2.735294117647059</v>
       </c>
     </row>
     <row r="4">
@@ -665,61 +665,61 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.392761625776845</v>
+        <v>1.377499348939224</v>
       </c>
       <c r="C4" t="n">
-        <v>1.362319337928748</v>
+        <v>1.308480497417219</v>
       </c>
       <c r="D4" t="n">
-        <v>1.448766624126466</v>
+        <v>1.466500557762595</v>
       </c>
       <c r="E4" t="n">
-        <v>1.668171363776735</v>
+        <v>1.665685985989427</v>
       </c>
       <c r="F4" t="n">
-        <v>1.340036911704742</v>
+        <v>1.347077115755897</v>
       </c>
       <c r="G4" t="n">
-        <v>1.482514574082019</v>
+        <v>1.453988306842575</v>
       </c>
       <c r="H4" t="n">
-        <v>1.557500064723242</v>
+        <v>1.54781197990379</v>
       </c>
       <c r="I4" t="n">
-        <v>1.521883383264981</v>
+        <v>1.479810654169145</v>
       </c>
       <c r="J4" t="n">
-        <v>1.398924317935687</v>
+        <v>1.381053358091791</v>
       </c>
       <c r="K4" t="n">
-        <v>1.465003945093591</v>
+        <v>1.432995441663677</v>
       </c>
       <c r="L4" t="n">
-        <v>1.279280711878728</v>
+        <v>1.248528545693596</v>
       </c>
       <c r="M4" t="n">
-        <v>1.353609273208532</v>
+        <v>1.381053358091791</v>
       </c>
       <c r="N4" t="n">
-        <v>1.4308430479815</v>
+        <v>1.43827238414022</v>
       </c>
       <c r="O4" t="n">
-        <v>1.202148614075057</v>
+        <v>1.173458711499294</v>
       </c>
       <c r="P4" t="n">
-        <v>1.282638409811035</v>
+        <v>1.365803388057981</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.204828993353748</v>
+        <v>1.181029491391532</v>
       </c>
       <c r="R4" t="n">
-        <v>1.45985711482286</v>
+        <v>1.429570569877629</v>
       </c>
       <c r="S4" t="n">
-        <v>1.355197085218584</v>
+        <v>1.328422328310143</v>
       </c>
       <c r="T4" t="n">
-        <v>1.585553056388734</v>
+        <v>1.54348726628258</v>
       </c>
     </row>
     <row r="5">
@@ -814,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J6" t="n">
         <v>2</v>
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="Q6" t="n">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="R6" t="n">
         <v>2</v>
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
         <v>4</v>
@@ -866,19 +866,19 @@
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="J7" t="n">
         <v>3</v>
@@ -887,10 +887,10 @@
         <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="N7" t="n">
         <v>3</v>
@@ -905,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="R7" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S7" t="n">
         <v>4</v>
@@ -924,13 +924,13 @@
         <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="D8" t="n">
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="F8" t="n">
         <v>4</v>
@@ -957,13 +957,13 @@
         <v>4</v>
       </c>
       <c r="N8" t="n">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="O8" t="n">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="P8" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="Q8" t="n">
         <v>4</v>
@@ -972,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="S8" t="n">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="T8" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Prepared tables / charts and data to write the final chapter
</commit_message>
<xml_diff>
--- a/wyniki/AI_statistics.xlsx
+++ b/wyniki/AI_statistics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,16 +519,6 @@
           <t>I play longer than I meant to_16</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>I really get into the game_17</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>I feel like I just can't stop playing_18</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -587,12 +577,6 @@
       <c r="R2" t="n">
         <v>34</v>
       </c>
-      <c r="S2" t="n">
-        <v>34</v>
-      </c>
-      <c r="T2" t="n">
-        <v>34</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -651,12 +635,6 @@
       <c r="R3" t="n">
         <v>3.323529411764706</v>
       </c>
-      <c r="S3" t="n">
-        <v>3.411764705882353</v>
-      </c>
-      <c r="T3" t="n">
-        <v>2.735294117647059</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -715,12 +693,6 @@
       <c r="R4" t="n">
         <v>1.429570569877629</v>
       </c>
-      <c r="S4" t="n">
-        <v>1.328422328310143</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1.54348726628258</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -779,12 +751,6 @@
       <c r="R5" t="n">
         <v>1</v>
       </c>
-      <c r="S5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -843,12 +809,6 @@
       <c r="R6" t="n">
         <v>2</v>
       </c>
-      <c r="S6" t="n">
-        <v>2</v>
-      </c>
-      <c r="T6" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -907,12 +867,6 @@
       <c r="R7" t="n">
         <v>3.5</v>
       </c>
-      <c r="S7" t="n">
-        <v>4</v>
-      </c>
-      <c r="T7" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -971,12 +925,6 @@
       <c r="R8" t="n">
         <v>5</v>
       </c>
-      <c r="S8" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="T8" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1033,12 +981,6 @@
         <v>5</v>
       </c>
       <c r="R9" t="n">
-        <v>5</v>
-      </c>
-      <c r="S9" t="n">
-        <v>5</v>
-      </c>
-      <c r="T9" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>